<commit_message>
ex06 - P1 coding done
</commit_message>
<xml_diff>
--- a/ex06/ex06.xlsx
+++ b/ex06/ex06.xlsx
@@ -5,15 +5,16 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\CSE\CSMC\ex06\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\CSE\CSMC\CSMC_2021WS\ex06\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCD65E58-09CB-453D-A83E-ED8625369393}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE2E3BB9-0442-42F6-BFDA-81C9672A913C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="16080" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Prefix sum" sheetId="3" r:id="rId1"/>
+    <sheet name="Part1_timings" sheetId="4" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="14">
   <si>
     <t>grid level</t>
   </si>
@@ -59,12 +60,30 @@
   <si>
     <t>so if every thread knows its number of entries - a prefix sum will do the trick. But… do we now need as many threads, as we have rows?</t>
   </si>
+  <si>
+    <t>exlcusive scan</t>
+  </si>
+  <si>
+    <t>inclusidve scan 1</t>
+  </si>
+  <si>
+    <t>inclusidve scan 2</t>
+  </si>
+  <si>
+    <t>300000000;5.08280000e-02</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> elapsed time in s</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -78,6 +97,11 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial Unicode MS"/>
     </font>
   </fonts>
   <fills count="3">
@@ -351,7 +375,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -393,6 +417,10 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -408,6 +436,1305 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.15962072072471595"/>
+          <c:y val="5.0925925925925923E-2"/>
+          <c:w val="0.77534449478372414"/>
+          <c:h val="0.78877265849749645"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Part1_timings!$G$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>exlcusive scan</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:prstDash val="dash"/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Part1_timings!$F$4:$F$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>30000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>100000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>300000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1000000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3000000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>10000000</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>30000000</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>100000000</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>300000000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Part1_timings!$G$4:$G$13</c:f>
+              <c:numCache>
+                <c:formatCode>0.00E+00</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>1.8000000000000001E-4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.8000000000000001E-4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.9100000000000003E-4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8.0999999999999996E-4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.0769999999999999E-3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6.1069999999999996E-3</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.983E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>7.3550000000000004E-3</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.9449000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>5.1249000000000003E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-D7DE-4C0B-B1D1-650A0FEABFD6}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Part1_timings!$H$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>inclusidve scan 1</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Part1_timings!$F$4:$F$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>30000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>100000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>300000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1000000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3000000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>10000000</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>30000000</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>100000000</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>300000000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Part1_timings!$H$4:$H$13</c:f>
+              <c:numCache>
+                <c:formatCode>0.00E+00</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>1.95E-4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.9900000000000001E-4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.1700000000000001E-4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8.6499999999999999E-4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.258E-3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6.4120000000000002E-3</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.2017999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>9.3179999999999999E-3</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2.4944999999999998E-2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>7.2107000000000004E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-D7DE-4C0B-B1D1-650A0FEABFD6}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Part1_timings!$I$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>inclusidve scan 2</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:prstDash val="sysDot"/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Part1_timings!$F$4:$F$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>30000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>100000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>300000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1000000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3000000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>10000000</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>30000000</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>100000000</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>300000000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Part1_timings!$I$4:$I$13</c:f>
+              <c:numCache>
+                <c:formatCode>0.00E+00</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>1.75E-4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.7799999999999999E-4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.9100000000000003E-4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8.0400000000000003E-4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.0699999999999998E-3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5.8799999999999998E-3</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.9939999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>7.1450000000000003E-3</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.7895000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>5.0827999999999998E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-D7DE-4C0B-B1D1-650A0FEABFD6}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="2102002176"/>
+        <c:axId val="2102004256"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="2102002176"/>
+        <c:scaling>
+          <c:logBase val="10"/>
+          <c:orientation val="minMax"/>
+          <c:min val="1000"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>vector size</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="0.E+00" sourceLinked="0"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2102004256"/>
+        <c:crossesAt val="1.0000000000000003E-4"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="2102004256"/>
+        <c:scaling>
+          <c:logBase val="10"/>
+          <c:orientation val="minMax"/>
+          <c:max val="0.1"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>execution time in s</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="0.E+00" sourceLinked="0"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2102002176"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.19319588698284326"/>
+          <c:y val="9.4405429080520409E-2"/>
+          <c:w val="0.29781386701662299"/>
+          <c:h val="0.31584153734359288"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1138,6 +2465,47 @@
         </a:fontRef>
       </xdr:style>
     </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>300036</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>147637</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>609599</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0B13DCBB-D622-4E26-AF12-5154AC3913E5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -1409,16 +2777,16 @@
   <dimension ref="H4:AX38"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="O4" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="AI17" sqref="AI17"/>
+      <selection activeCell="W19" sqref="W19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="2.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="2.7109375" defaultRowHeight="15"/>
   <cols>
     <col min="11" max="15" width="3" bestFit="1" customWidth="1"/>
     <col min="23" max="27" width="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="8:50" x14ac:dyDescent="0.25">
+    <row r="4" spans="8:50">
       <c r="AE4">
         <v>1</v>
       </c>
@@ -1444,8 +2812,8 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="8:50" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="6" spans="8:50" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="8:50" ht="15.75" thickBot="1"/>
+    <row r="6" spans="8:50" ht="15.75" thickBot="1">
       <c r="H6">
         <v>1</v>
       </c>
@@ -1511,8 +2879,8 @@
       <c r="AW6" s="19"/>
       <c r="AX6" s="7"/>
     </row>
-    <row r="7" spans="8:50" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="8" spans="8:50" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="8:50" ht="15.75" thickBot="1"/>
+    <row r="8" spans="8:50" ht="15.75" thickBot="1">
       <c r="AQ8" s="2"/>
       <c r="AR8" s="9"/>
       <c r="AS8" s="2"/>
@@ -1522,7 +2890,7 @@
       <c r="AW8" s="2"/>
       <c r="AX8" s="7"/>
     </row>
-    <row r="9" spans="8:50" x14ac:dyDescent="0.25">
+    <row r="9" spans="8:50">
       <c r="H9" s="1">
         <v>1</v>
       </c>
@@ -1580,8 +2948,8 @@
       <c r="AK9" s="6"/>
       <c r="AL9" s="7"/>
     </row>
-    <row r="10" spans="8:50" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="11" spans="8:50" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="8:50" ht="15.75" thickBot="1"/>
+    <row r="11" spans="8:50" ht="15.75" thickBot="1">
       <c r="AQ11" s="21"/>
       <c r="AR11" s="5"/>
       <c r="AS11" s="19"/>
@@ -1591,7 +2959,7 @@
       <c r="AW11" s="19"/>
       <c r="AX11" s="7"/>
     </row>
-    <row r="12" spans="8:50" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="8:50" ht="15.75" thickBot="1">
       <c r="H12" s="1">
         <v>1</v>
       </c>
@@ -1641,7 +3009,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="13" spans="8:50" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="8:50" ht="15.75" thickBot="1">
       <c r="AQ13" s="6"/>
       <c r="AR13" s="8"/>
       <c r="AS13" s="2"/>
@@ -1651,7 +3019,7 @@
       <c r="AW13" s="2"/>
       <c r="AX13" s="7"/>
     </row>
-    <row r="15" spans="8:50" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="8:50" ht="15.75" thickBot="1">
       <c r="H15" s="1">
         <v>1</v>
       </c>
@@ -1709,7 +3077,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="16" spans="8:50" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="8:50" ht="15.75" thickBot="1">
       <c r="AQ16" s="4"/>
       <c r="AR16" s="5"/>
       <c r="AS16" s="20"/>
@@ -1719,8 +3087,8 @@
       <c r="AW16" s="19"/>
       <c r="AX16" s="7"/>
     </row>
-    <row r="17" spans="8:50" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="18" spans="8:50" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="8:50" ht="15.75" thickBot="1"/>
+    <row r="18" spans="8:50" ht="15.75" thickBot="1">
       <c r="AQ18" s="6"/>
       <c r="AR18" s="6"/>
       <c r="AS18" s="6"/>
@@ -1730,17 +3098,17 @@
       <c r="AW18" s="2"/>
       <c r="AX18" s="7"/>
     </row>
-    <row r="20" spans="8:50" x14ac:dyDescent="0.25">
+    <row r="20" spans="8:50">
       <c r="H20" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="8:50" x14ac:dyDescent="0.25">
+    <row r="22" spans="8:50">
       <c r="H22" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="8:50" x14ac:dyDescent="0.25">
+    <row r="27" spans="8:50">
       <c r="H27" t="s">
         <v>2</v>
       </c>
@@ -1748,12 +3116,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="29" spans="8:50" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="8:50" ht="15.75" thickBot="1">
       <c r="P29" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="30" spans="8:50" x14ac:dyDescent="0.25">
+    <row r="30" spans="8:50">
       <c r="H30" s="10"/>
       <c r="I30" s="11">
         <v>2</v>
@@ -1793,7 +3161,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="31" spans="8:50" x14ac:dyDescent="0.25">
+    <row r="31" spans="8:50">
       <c r="H31" s="13"/>
       <c r="I31" s="14"/>
       <c r="J31" s="14">
@@ -1804,7 +3172,7 @@
       </c>
       <c r="L31" s="15"/>
     </row>
-    <row r="32" spans="8:50" x14ac:dyDescent="0.25">
+    <row r="32" spans="8:50">
       <c r="H32" s="13">
         <v>3</v>
       </c>
@@ -1816,7 +3184,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="33" spans="8:24" x14ac:dyDescent="0.25">
+    <row r="33" spans="8:24">
       <c r="H33" s="13"/>
       <c r="I33" s="14"/>
       <c r="J33" s="14">
@@ -1854,7 +3222,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="8:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="8:24" ht="15.75" thickBot="1">
       <c r="H34" s="16"/>
       <c r="I34" s="17">
         <v>8</v>
@@ -1863,12 +3231,12 @@
       <c r="K34" s="17"/>
       <c r="L34" s="18"/>
     </row>
-    <row r="35" spans="8:24" x14ac:dyDescent="0.25">
+    <row r="35" spans="8:24">
       <c r="P35" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="36" spans="8:24" x14ac:dyDescent="0.25">
+    <row r="36" spans="8:24">
       <c r="P36">
         <v>0</v>
       </c>
@@ -1888,10 +3256,491 @@
         <v>9</v>
       </c>
     </row>
-    <row r="38" spans="8:24" x14ac:dyDescent="0.25">
+    <row r="38" spans="8:24">
       <c r="P38" t="s">
         <v>7</v>
       </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48E9978B-894D-45BE-8A10-ACBB05A286EC}">
+  <dimension ref="A1:I41"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G29" sqref="G29"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:9">
+      <c r="A1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
+      <c r="A2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
+      <c r="A3" s="23">
+        <v>10000</v>
+      </c>
+      <c r="B3" s="24">
+        <v>1.8000000000000001E-4</v>
+      </c>
+      <c r="F3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G3" t="s">
+        <v>8</v>
+      </c>
+      <c r="H3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
+      <c r="A4" s="23">
+        <v>30000</v>
+      </c>
+      <c r="B4" s="24">
+        <v>1.8000000000000001E-4</v>
+      </c>
+      <c r="F4" s="23">
+        <v>10000</v>
+      </c>
+      <c r="G4" s="24">
+        <v>1.8000000000000001E-4</v>
+      </c>
+      <c r="H4" s="24">
+        <v>1.95E-4</v>
+      </c>
+      <c r="I4" s="24">
+        <v>1.75E-4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
+      <c r="A5" s="23">
+        <v>100000</v>
+      </c>
+      <c r="B5" s="24">
+        <v>2.9100000000000003E-4</v>
+      </c>
+      <c r="F5" s="23">
+        <v>30000</v>
+      </c>
+      <c r="G5" s="24">
+        <v>1.8000000000000001E-4</v>
+      </c>
+      <c r="H5" s="24">
+        <v>1.9900000000000001E-4</v>
+      </c>
+      <c r="I5" s="24">
+        <v>1.7799999999999999E-4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
+      <c r="A6" s="23">
+        <v>300000</v>
+      </c>
+      <c r="B6" s="24">
+        <v>8.0999999999999996E-4</v>
+      </c>
+      <c r="F6" s="23">
+        <v>100000</v>
+      </c>
+      <c r="G6" s="24">
+        <v>2.9100000000000003E-4</v>
+      </c>
+      <c r="H6" s="24">
+        <v>3.1700000000000001E-4</v>
+      </c>
+      <c r="I6" s="24">
+        <v>2.9100000000000003E-4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
+      <c r="A7" s="23">
+        <v>1000000</v>
+      </c>
+      <c r="B7" s="24">
+        <v>2.0769999999999999E-3</v>
+      </c>
+      <c r="F7" s="23">
+        <v>300000</v>
+      </c>
+      <c r="G7" s="24">
+        <v>8.0999999999999996E-4</v>
+      </c>
+      <c r="H7" s="24">
+        <v>8.6499999999999999E-4</v>
+      </c>
+      <c r="I7" s="24">
+        <v>8.0400000000000003E-4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9">
+      <c r="A8" s="23">
+        <v>3000000</v>
+      </c>
+      <c r="B8" s="24">
+        <v>6.1069999999999996E-3</v>
+      </c>
+      <c r="F8" s="23">
+        <v>1000000</v>
+      </c>
+      <c r="G8" s="24">
+        <v>2.0769999999999999E-3</v>
+      </c>
+      <c r="H8" s="24">
+        <v>2.258E-3</v>
+      </c>
+      <c r="I8" s="24">
+        <v>2.0699999999999998E-3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9">
+      <c r="A9" s="23">
+        <v>10000000</v>
+      </c>
+      <c r="B9" s="24">
+        <v>1.983E-2</v>
+      </c>
+      <c r="F9" s="23">
+        <v>3000000</v>
+      </c>
+      <c r="G9" s="24">
+        <v>6.1069999999999996E-3</v>
+      </c>
+      <c r="H9" s="24">
+        <v>6.4120000000000002E-3</v>
+      </c>
+      <c r="I9" s="24">
+        <v>5.8799999999999998E-3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9">
+      <c r="A10" s="23">
+        <v>30000000</v>
+      </c>
+      <c r="B10" s="24">
+        <v>7.3550000000000004E-3</v>
+      </c>
+      <c r="F10" s="23">
+        <v>10000000</v>
+      </c>
+      <c r="G10" s="24">
+        <v>1.983E-2</v>
+      </c>
+      <c r="H10" s="24">
+        <v>2.2017999999999999E-2</v>
+      </c>
+      <c r="I10" s="24">
+        <v>1.9939999999999999E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9">
+      <c r="A11" s="23">
+        <v>100000000</v>
+      </c>
+      <c r="B11" s="24">
+        <v>1.9449000000000001E-2</v>
+      </c>
+      <c r="F11" s="23">
+        <v>30000000</v>
+      </c>
+      <c r="G11" s="24">
+        <v>7.3550000000000004E-3</v>
+      </c>
+      <c r="H11" s="24">
+        <v>9.3179999999999999E-3</v>
+      </c>
+      <c r="I11" s="24">
+        <v>7.1450000000000003E-3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9">
+      <c r="A12" s="23">
+        <v>300000000</v>
+      </c>
+      <c r="B12" s="24">
+        <v>5.1249000000000003E-2</v>
+      </c>
+      <c r="F12" s="23">
+        <v>100000000</v>
+      </c>
+      <c r="G12" s="24">
+        <v>1.9449000000000001E-2</v>
+      </c>
+      <c r="H12" s="24">
+        <v>2.4944999999999998E-2</v>
+      </c>
+      <c r="I12" s="24">
+        <v>1.7895000000000001E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9">
+      <c r="A13" s="23"/>
+      <c r="F13" s="23">
+        <v>300000000</v>
+      </c>
+      <c r="G13" s="24">
+        <v>5.1249000000000003E-2</v>
+      </c>
+      <c r="H13" s="24">
+        <v>7.2107000000000004E-2</v>
+      </c>
+      <c r="I13" s="24">
+        <v>5.0827999999999998E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9">
+      <c r="A14" t="s">
+        <v>9</v>
+      </c>
+      <c r="F14" s="23"/>
+    </row>
+    <row r="15" spans="1:9">
+      <c r="A15" s="23" t="s">
+        <v>12</v>
+      </c>
+      <c r="B15" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9">
+      <c r="A16" s="23">
+        <v>10000</v>
+      </c>
+      <c r="B16" s="24">
+        <v>1.95E-4</v>
+      </c>
+      <c r="F16" s="23"/>
+    </row>
+    <row r="17" spans="1:7">
+      <c r="A17" s="23">
+        <v>30000</v>
+      </c>
+      <c r="B17" s="24">
+        <v>1.9900000000000001E-4</v>
+      </c>
+      <c r="F17" s="23"/>
+    </row>
+    <row r="18" spans="1:7">
+      <c r="A18" s="23">
+        <v>100000</v>
+      </c>
+      <c r="B18" s="24">
+        <v>3.1700000000000001E-4</v>
+      </c>
+      <c r="F18" s="23"/>
+    </row>
+    <row r="19" spans="1:7">
+      <c r="A19" s="23">
+        <v>300000</v>
+      </c>
+      <c r="B19" s="24">
+        <v>8.6499999999999999E-4</v>
+      </c>
+      <c r="F19" s="23"/>
+    </row>
+    <row r="20" spans="1:7">
+      <c r="A20" s="23">
+        <v>1000000</v>
+      </c>
+      <c r="B20" s="24">
+        <v>2.258E-3</v>
+      </c>
+      <c r="F20" s="23"/>
+    </row>
+    <row r="21" spans="1:7">
+      <c r="A21" s="23">
+        <v>3000000</v>
+      </c>
+      <c r="B21" s="24">
+        <v>6.4120000000000002E-3</v>
+      </c>
+      <c r="F21" s="23"/>
+    </row>
+    <row r="22" spans="1:7">
+      <c r="A22" s="23">
+        <v>10000000</v>
+      </c>
+      <c r="B22" s="24">
+        <v>2.2017999999999999E-2</v>
+      </c>
+      <c r="F22" s="23"/>
+    </row>
+    <row r="23" spans="1:7">
+      <c r="A23" s="23">
+        <v>30000000</v>
+      </c>
+      <c r="B23" s="24">
+        <v>9.3179999999999999E-3</v>
+      </c>
+      <c r="F23" s="23"/>
+    </row>
+    <row r="24" spans="1:7">
+      <c r="A24" s="23">
+        <v>100000000</v>
+      </c>
+      <c r="B24" s="24">
+        <v>2.4944999999999998E-2</v>
+      </c>
+      <c r="F24" s="23"/>
+    </row>
+    <row r="25" spans="1:7">
+      <c r="A25" s="23">
+        <v>300000000</v>
+      </c>
+      <c r="B25" s="24">
+        <v>7.2107000000000004E-2</v>
+      </c>
+      <c r="F25" s="23"/>
+    </row>
+    <row r="26" spans="1:7">
+      <c r="A26" s="23"/>
+      <c r="F26" s="23"/>
+    </row>
+    <row r="27" spans="1:7">
+      <c r="F27" s="23"/>
+    </row>
+    <row r="28" spans="1:7">
+      <c r="A28" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7">
+      <c r="A29" s="23" t="s">
+        <v>12</v>
+      </c>
+      <c r="B29" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7">
+      <c r="A30" s="23">
+        <v>10000</v>
+      </c>
+      <c r="B30" s="24">
+        <v>1.75E-4</v>
+      </c>
+      <c r="F30" s="23"/>
+    </row>
+    <row r="31" spans="1:7">
+      <c r="A31" s="23">
+        <v>30000</v>
+      </c>
+      <c r="B31" s="24">
+        <v>1.7799999999999999E-4</v>
+      </c>
+      <c r="F31" s="23"/>
+      <c r="G31" s="24"/>
+    </row>
+    <row r="32" spans="1:7">
+      <c r="A32" s="23">
+        <v>100000</v>
+      </c>
+      <c r="B32" s="24">
+        <v>2.9100000000000003E-4</v>
+      </c>
+      <c r="F32" s="23"/>
+      <c r="G32" s="24"/>
+    </row>
+    <row r="33" spans="1:7">
+      <c r="A33" s="23">
+        <v>300000</v>
+      </c>
+      <c r="B33" s="24">
+        <v>8.0400000000000003E-4</v>
+      </c>
+      <c r="F33" s="23"/>
+      <c r="G33" s="24"/>
+    </row>
+    <row r="34" spans="1:7">
+      <c r="A34" s="23">
+        <v>1000000</v>
+      </c>
+      <c r="B34" s="24">
+        <v>2.0699999999999998E-3</v>
+      </c>
+      <c r="F34" s="23"/>
+      <c r="G34" s="24"/>
+    </row>
+    <row r="35" spans="1:7">
+      <c r="A35" s="23">
+        <v>3000000</v>
+      </c>
+      <c r="B35" s="24">
+        <v>5.8799999999999998E-3</v>
+      </c>
+      <c r="F35" s="23"/>
+      <c r="G35" s="24"/>
+    </row>
+    <row r="36" spans="1:7">
+      <c r="A36" s="23">
+        <v>10000000</v>
+      </c>
+      <c r="B36" s="24">
+        <v>1.9939999999999999E-2</v>
+      </c>
+      <c r="F36" s="23"/>
+      <c r="G36" s="24"/>
+    </row>
+    <row r="37" spans="1:7">
+      <c r="A37" s="23">
+        <v>30000000</v>
+      </c>
+      <c r="B37" s="24">
+        <v>7.1450000000000003E-3</v>
+      </c>
+      <c r="F37" s="23"/>
+      <c r="G37" s="24"/>
+    </row>
+    <row r="38" spans="1:7">
+      <c r="A38" s="23">
+        <v>100000000</v>
+      </c>
+      <c r="B38" s="24">
+        <v>1.7895000000000001E-2</v>
+      </c>
+      <c r="F38" s="23"/>
+      <c r="G38" s="24"/>
+    </row>
+    <row r="39" spans="1:7">
+      <c r="A39" s="23">
+        <v>300000000</v>
+      </c>
+      <c r="B39" s="24">
+        <v>5.0827999999999998E-2</v>
+      </c>
+      <c r="F39" s="23"/>
+      <c r="G39" s="24"/>
+    </row>
+    <row r="40" spans="1:7">
+      <c r="A40" s="23" t="s">
+        <v>11</v>
+      </c>
+      <c r="F40" s="23"/>
+      <c r="G40" s="24"/>
+    </row>
+    <row r="41" spans="1:7">
+      <c r="F41" s="23"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
ex06 - P1 done and documented
</commit_message>
<xml_diff>
--- a/ex06/ex06.xlsx
+++ b/ex06/ex06.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\CSE\CSMC\CSMC_2021WS\ex06\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE2E3BB9-0442-42F6-BFDA-81C9672A913C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BF9FA92-7C4F-4676-87D1-9B8A28C7CA17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="16080" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Prefix sum" sheetId="3" r:id="rId1"/>
-    <sheet name="Part1_timings" sheetId="4" r:id="rId2"/>
+    <sheet name="Kernel1" sheetId="5" r:id="rId2"/>
+    <sheet name="Part1_timings" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="30">
   <si>
     <t>grid level</t>
   </si>
@@ -78,6 +79,54 @@
   <si>
     <t xml:space="preserve"> elapsed time in s</t>
   </si>
+  <si>
+    <t>vector divided in as many sections as there are blocks</t>
+  </si>
+  <si>
+    <t>section divided in as many subsections, as needed</t>
+  </si>
+  <si>
+    <t>subsection size = number of threads per block</t>
+  </si>
+  <si>
+    <t>output vector</t>
+  </si>
+  <si>
+    <t>input vector</t>
+  </si>
+  <si>
+    <t>separate prefix sum</t>
+  </si>
+  <si>
+    <t>carries</t>
+  </si>
+  <si>
+    <t>sum over sections</t>
+  </si>
+  <si>
+    <t>sum1</t>
+  </si>
+  <si>
+    <t>sum2</t>
+  </si>
+  <si>
+    <t>sum1 + sum2</t>
+  </si>
+  <si>
+    <t>already done</t>
+  </si>
+  <si>
+    <t>add to each entry</t>
+  </si>
+  <si>
+    <t>stride = 1</t>
+  </si>
+  <si>
+    <t>stride = 2</t>
+  </si>
+  <si>
+    <t>stride = 4</t>
+  </si>
 </sst>
 </file>
 
@@ -118,7 +167,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="18">
+  <borders count="23">
     <border>
       <left/>
       <right/>
@@ -371,11 +420,74 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="dotted">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -421,6 +533,17 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2474,6 +2597,648 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>20839</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>47626</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>5955</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>181572</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="Right Brace 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{827994C7-0E4E-4B5C-A57B-860FF10A028F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="16200000">
+          <a:off x="2714628" y="2330650"/>
+          <a:ext cx="133946" cy="520897"/>
+        </a:xfrm>
+        <a:prstGeom prst="rightBrace">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="12700">
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-GB" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>2</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>35719</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>31</xdr:col>
+      <xdr:colOff>142875</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="Right Brace 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5E212B16-7E34-47B1-B68C-81E0BC8E7AA8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="16200000">
+          <a:off x="3184923" y="-160733"/>
+          <a:ext cx="202406" cy="4786310"/>
+        </a:xfrm>
+        <a:prstGeom prst="rightBrace">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="12700">
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-GB" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>5955</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>53577</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>2</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>32740</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="4" name="Right Brace 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E795BC36-853A-4586-B27F-0D089ABB246C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="16200000" flipH="1">
+          <a:off x="3222131" y="2219027"/>
+          <a:ext cx="169663" cy="1601390"/>
+        </a:xfrm>
+        <a:prstGeom prst="rightBrace">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="12700">
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-GB" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>53579</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>154781</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>53579</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>107156</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="10" name="Straight Arrow Connector 9">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2D1116E4-4A30-4002-B5F3-7EE52FB46808}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2732485" y="4774406"/>
+          <a:ext cx="0" cy="333375"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="25400">
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+          <a:tailEnd type="arrow" w="med" len="med"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>53578</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>154781</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>53578</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>107156</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="11" name="Straight Arrow Connector 10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E13F9179-D30B-4EF5-A485-CBE00D128108}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4339828" y="4774406"/>
+          <a:ext cx="0" cy="333375"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="25400">
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+          <a:tailEnd type="arrow" w="med" len="med"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>53578</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>154781</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>53578</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>107156</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="12" name="Straight Arrow Connector 11">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DCE37B8D-95A4-4C5F-8689-689F26A7F314}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1125141" y="4774406"/>
+          <a:ext cx="0" cy="333375"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="25400">
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+          <a:tailEnd type="arrow" w="med" len="med"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>119062</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>83345</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>30</xdr:col>
+      <xdr:colOff>172640</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>184546</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="44" name="Straight Arrow Connector 43">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7E77F361-DDDE-4753-8E15-485D76131E68}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="1905000" y="4512470"/>
+          <a:ext cx="3625453" cy="696514"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="25400">
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+          <a:tailEnd type="arrow" w="med" len="med"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>130968</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>31</xdr:col>
+      <xdr:colOff>11906</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>5953</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="47" name="Straight Arrow Connector 46">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C635DC61-2095-4DBE-BE83-8FCF8707F6C0}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="3345656" y="4726781"/>
+          <a:ext cx="2202656" cy="506016"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="25400">
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+          <a:tailEnd type="arrow" w="med" len="med"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>148827</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>23812</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>101203</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="51" name="Straight Arrow Connector 50">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{57852E48-CD0C-461F-B30F-D2322ECC3702}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2649140" y="8048625"/>
+          <a:ext cx="589360" cy="5953"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="25400">
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+          <a:tailEnd type="arrow" w="med" len="med"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>130969</xdr:colOff>
+      <xdr:row>52</xdr:row>
+      <xdr:rowOff>107156</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>32</xdr:col>
+      <xdr:colOff>113109</xdr:colOff>
+      <xdr:row>55</xdr:row>
+      <xdr:rowOff>125015</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="53" name="Straight Arrow Connector 52">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BD7C7E91-7F52-463C-B373-340E58B79AAC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="3881438" y="10203656"/>
+          <a:ext cx="1946671" cy="613172"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="25400">
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+          <a:tailEnd type="arrow" w="med" len="med"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>30</xdr:col>
+      <xdr:colOff>107156</xdr:colOff>
+      <xdr:row>53</xdr:row>
+      <xdr:rowOff>166688</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>32</xdr:col>
+      <xdr:colOff>113109</xdr:colOff>
+      <xdr:row>55</xdr:row>
+      <xdr:rowOff>125015</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="56" name="Straight Arrow Connector 55">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B200CEC1-0782-4B37-886F-FBAF2E724C71}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="5464969" y="10465594"/>
+          <a:ext cx="363140" cy="351234"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="25400">
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+          <a:tailEnd type="arrow" w="med" len="med"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
       <xdr:col>10</xdr:col>
       <xdr:colOff>300036</xdr:colOff>
       <xdr:row>4</xdr:row>
@@ -2774,10 +3539,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F3F8FFA-9A53-4E7A-B7DD-1557C851762A}">
-  <dimension ref="H4:AX38"/>
+  <dimension ref="H4:BA38"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="O4" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="W19" sqref="W19"/>
+    <sheetView showGridLines="0" topLeftCell="D3" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="AG18" sqref="AG18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.7109375" defaultRowHeight="15"/>
@@ -2786,7 +3551,7 @@
     <col min="23" max="27" width="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="8:50">
+    <row r="4" spans="8:53">
       <c r="AE4">
         <v>1</v>
       </c>
@@ -2812,8 +3577,8 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="8:50" ht="15.75" thickBot="1"/>
-    <row r="6" spans="8:50" ht="15.75" thickBot="1">
+    <row r="5" spans="8:53" ht="15.75" thickBot="1"/>
+    <row r="6" spans="8:53" ht="15.75" thickBot="1">
       <c r="H6">
         <v>1</v>
       </c>
@@ -2878,9 +3643,12 @@
       <c r="AV6" s="21"/>
       <c r="AW6" s="19"/>
       <c r="AX6" s="7"/>
-    </row>
-    <row r="7" spans="8:50" ht="15.75" thickBot="1"/>
-    <row r="8" spans="8:50" ht="15.75" thickBot="1">
+      <c r="BA6" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="7" spans="8:53" ht="15.75" thickBot="1"/>
+    <row r="8" spans="8:53" ht="15.75" thickBot="1">
       <c r="AQ8" s="2"/>
       <c r="AR8" s="9"/>
       <c r="AS8" s="2"/>
@@ -2890,7 +3658,7 @@
       <c r="AW8" s="2"/>
       <c r="AX8" s="7"/>
     </row>
-    <row r="9" spans="8:50">
+    <row r="9" spans="8:53">
       <c r="H9" s="1">
         <v>1</v>
       </c>
@@ -2948,8 +3716,8 @@
       <c r="AK9" s="6"/>
       <c r="AL9" s="7"/>
     </row>
-    <row r="10" spans="8:50" ht="15.75" thickBot="1"/>
-    <row r="11" spans="8:50" ht="15.75" thickBot="1">
+    <row r="10" spans="8:53" ht="15.75" thickBot="1"/>
+    <row r="11" spans="8:53" ht="15.75" thickBot="1">
       <c r="AQ11" s="21"/>
       <c r="AR11" s="5"/>
       <c r="AS11" s="19"/>
@@ -2958,8 +3726,11 @@
       <c r="AV11" s="5"/>
       <c r="AW11" s="19"/>
       <c r="AX11" s="7"/>
-    </row>
-    <row r="12" spans="8:50" ht="15.75" thickBot="1">
+      <c r="BA11" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="12" spans="8:53" ht="15.75" thickBot="1">
       <c r="H12" s="1">
         <v>1</v>
       </c>
@@ -3009,7 +3780,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="13" spans="8:50" ht="15.75" thickBot="1">
+    <row r="13" spans="8:53" ht="15.75" thickBot="1">
       <c r="AQ13" s="6"/>
       <c r="AR13" s="8"/>
       <c r="AS13" s="2"/>
@@ -3019,7 +3790,7 @@
       <c r="AW13" s="2"/>
       <c r="AX13" s="7"/>
     </row>
-    <row r="15" spans="8:50" ht="15.75" thickBot="1">
+    <row r="15" spans="8:53" ht="15.75" thickBot="1">
       <c r="H15" s="1">
         <v>1</v>
       </c>
@@ -3077,7 +3848,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="16" spans="8:50" ht="15.75" thickBot="1">
+    <row r="16" spans="8:53" ht="15.75" thickBot="1">
       <c r="AQ16" s="4"/>
       <c r="AR16" s="5"/>
       <c r="AS16" s="20"/>
@@ -3086,6 +3857,9 @@
       <c r="AV16" s="5"/>
       <c r="AW16" s="19"/>
       <c r="AX16" s="7"/>
+      <c r="BA16" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="17" spans="8:50" ht="15.75" thickBot="1"/>
     <row r="18" spans="8:50" ht="15.75" thickBot="1">
@@ -3269,11 +4043,461 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FBDD1BDF-C854-4E6E-A40A-935551068A3F}">
+  <dimension ref="F4:AQ57"/>
+  <sheetViews>
+    <sheetView showGridLines="0" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="W41" sqref="W41"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="2.7109375" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="4" spans="6:43">
+      <c r="F4">
+        <v>1</v>
+      </c>
+      <c r="G4">
+        <v>2</v>
+      </c>
+      <c r="H4">
+        <v>3</v>
+      </c>
+      <c r="I4">
+        <v>4</v>
+      </c>
+      <c r="J4">
+        <v>5</v>
+      </c>
+      <c r="K4">
+        <v>6</v>
+      </c>
+      <c r="L4">
+        <v>7</v>
+      </c>
+      <c r="M4">
+        <v>8</v>
+      </c>
+      <c r="N4">
+        <v>9</v>
+      </c>
+      <c r="O4">
+        <v>10</v>
+      </c>
+      <c r="P4">
+        <v>11</v>
+      </c>
+      <c r="Q4">
+        <v>12</v>
+      </c>
+      <c r="R4">
+        <v>13</v>
+      </c>
+      <c r="S4">
+        <v>14</v>
+      </c>
+      <c r="T4">
+        <v>15</v>
+      </c>
+      <c r="U4">
+        <v>16</v>
+      </c>
+      <c r="V4">
+        <v>17</v>
+      </c>
+      <c r="W4">
+        <v>18</v>
+      </c>
+      <c r="X4">
+        <v>19</v>
+      </c>
+      <c r="Y4">
+        <v>20</v>
+      </c>
+      <c r="Z4">
+        <v>21</v>
+      </c>
+      <c r="AA4">
+        <v>22</v>
+      </c>
+      <c r="AB4">
+        <v>23</v>
+      </c>
+      <c r="AC4">
+        <v>24</v>
+      </c>
+      <c r="AD4">
+        <v>25</v>
+      </c>
+      <c r="AE4">
+        <v>26</v>
+      </c>
+      <c r="AF4">
+        <v>27</v>
+      </c>
+      <c r="AG4">
+        <v>28</v>
+      </c>
+      <c r="AH4">
+        <v>29</v>
+      </c>
+      <c r="AI4">
+        <v>30</v>
+      </c>
+      <c r="AJ4">
+        <v>31</v>
+      </c>
+      <c r="AK4">
+        <v>32</v>
+      </c>
+      <c r="AL4">
+        <v>33</v>
+      </c>
+      <c r="AM4">
+        <v>34</v>
+      </c>
+      <c r="AN4">
+        <v>35</v>
+      </c>
+      <c r="AO4">
+        <v>36</v>
+      </c>
+      <c r="AP4">
+        <v>37</v>
+      </c>
+      <c r="AQ4">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="7" spans="6:43">
+      <c r="F7">
+        <v>1</v>
+      </c>
+      <c r="G7">
+        <v>2</v>
+      </c>
+      <c r="H7">
+        <v>3</v>
+      </c>
+      <c r="I7">
+        <v>4</v>
+      </c>
+      <c r="J7">
+        <v>5</v>
+      </c>
+      <c r="K7">
+        <v>6</v>
+      </c>
+      <c r="L7">
+        <v>7</v>
+      </c>
+      <c r="M7">
+        <v>8</v>
+      </c>
+      <c r="N7">
+        <v>9</v>
+      </c>
+      <c r="O7">
+        <v>1</v>
+      </c>
+      <c r="P7">
+        <v>2</v>
+      </c>
+      <c r="Q7">
+        <v>3</v>
+      </c>
+      <c r="R7">
+        <v>4</v>
+      </c>
+      <c r="S7">
+        <v>5</v>
+      </c>
+      <c r="T7">
+        <v>6</v>
+      </c>
+      <c r="U7">
+        <v>7</v>
+      </c>
+      <c r="V7">
+        <v>8</v>
+      </c>
+      <c r="W7">
+        <v>9</v>
+      </c>
+      <c r="X7">
+        <v>1</v>
+      </c>
+      <c r="Y7">
+        <v>2</v>
+      </c>
+      <c r="Z7">
+        <v>3</v>
+      </c>
+      <c r="AA7">
+        <v>4</v>
+      </c>
+      <c r="AB7">
+        <v>5</v>
+      </c>
+      <c r="AC7">
+        <v>6</v>
+      </c>
+      <c r="AD7">
+        <v>7</v>
+      </c>
+      <c r="AE7">
+        <v>8</v>
+      </c>
+      <c r="AF7">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="6:43">
+      <c r="S11" s="29" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="13" spans="6:43">
+      <c r="P13" s="29" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="14" spans="6:43" ht="15.75" thickBot="1"/>
+    <row r="15" spans="6:43" ht="15.75" thickBot="1">
+      <c r="F15" s="25"/>
+      <c r="G15" s="26"/>
+      <c r="H15" s="28"/>
+      <c r="I15" s="26"/>
+      <c r="J15" s="26"/>
+      <c r="K15" s="28"/>
+      <c r="L15" s="26"/>
+      <c r="M15" s="26"/>
+      <c r="N15" s="27"/>
+      <c r="O15" s="26"/>
+      <c r="P15" s="26"/>
+      <c r="Q15" s="28"/>
+      <c r="R15" s="26"/>
+      <c r="S15" s="26"/>
+      <c r="T15" s="28"/>
+      <c r="U15" s="26"/>
+      <c r="V15" s="26"/>
+      <c r="W15" s="27"/>
+      <c r="X15" s="26"/>
+      <c r="Y15" s="26"/>
+      <c r="Z15" s="28"/>
+      <c r="AA15" s="26"/>
+      <c r="AB15" s="26"/>
+      <c r="AC15" s="28"/>
+      <c r="AD15" s="26"/>
+      <c r="AE15" s="26"/>
+      <c r="AF15" s="3"/>
+    </row>
+    <row r="17" spans="6:34">
+      <c r="S17" s="29" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="22" spans="6:34" ht="15.75" thickBot="1"/>
+    <row r="23" spans="6:34" ht="15.75" thickBot="1">
+      <c r="AF23" s="30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="6:34" ht="15.75" thickBot="1">
+      <c r="V24" t="s">
+        <v>21</v>
+      </c>
+      <c r="AF24" s="2"/>
+      <c r="AH24" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="25" spans="6:34" ht="15.75" thickBot="1">
+      <c r="AF25" s="31"/>
+    </row>
+    <row r="27" spans="6:34" ht="15.75" thickBot="1"/>
+    <row r="28" spans="6:34" ht="15.75" thickBot="1">
+      <c r="F28" s="25"/>
+      <c r="G28" s="26"/>
+      <c r="H28" s="26"/>
+      <c r="I28" s="26"/>
+      <c r="J28" s="26"/>
+      <c r="K28" s="26"/>
+      <c r="L28" s="26"/>
+      <c r="M28" s="26"/>
+      <c r="N28" s="3"/>
+      <c r="O28" s="25"/>
+      <c r="P28" s="26"/>
+      <c r="Q28" s="26"/>
+      <c r="R28" s="26"/>
+      <c r="S28" s="26"/>
+      <c r="T28" s="26"/>
+      <c r="U28" s="26"/>
+      <c r="V28" s="26"/>
+      <c r="W28" s="3"/>
+      <c r="X28" s="26"/>
+      <c r="Y28" s="26"/>
+      <c r="Z28" s="26"/>
+      <c r="AA28" s="26"/>
+      <c r="AB28" s="26"/>
+      <c r="AC28" s="26"/>
+      <c r="AD28" s="26"/>
+      <c r="AE28" s="26"/>
+      <c r="AF28" s="3"/>
+      <c r="AH28" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="30" spans="6:34">
+      <c r="H30" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q30" t="s">
+        <v>19</v>
+      </c>
+      <c r="Z30" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="31" spans="6:34" ht="15.75" thickBot="1"/>
+    <row r="32" spans="6:34" ht="15.75" thickBot="1">
+      <c r="F32" s="25"/>
+      <c r="G32" s="26"/>
+      <c r="H32" s="26"/>
+      <c r="I32" s="26"/>
+      <c r="J32" s="26"/>
+      <c r="K32" s="26"/>
+      <c r="L32" s="26"/>
+      <c r="M32" s="26"/>
+      <c r="N32" s="3"/>
+      <c r="O32" s="25"/>
+      <c r="P32" s="26"/>
+      <c r="Q32" s="26"/>
+      <c r="R32" s="26"/>
+      <c r="S32" s="26"/>
+      <c r="T32" s="26"/>
+      <c r="U32" s="26"/>
+      <c r="V32" s="26"/>
+      <c r="W32" s="3"/>
+      <c r="X32" s="26"/>
+      <c r="Y32" s="26"/>
+      <c r="Z32" s="26"/>
+      <c r="AA32" s="26"/>
+      <c r="AB32" s="26"/>
+      <c r="AC32" s="26"/>
+      <c r="AD32" s="26"/>
+      <c r="AE32" s="26"/>
+      <c r="AF32" s="3"/>
+      <c r="AH32" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="40" spans="11:23" ht="15.75" thickBot="1"/>
+    <row r="41" spans="11:23" ht="15.75" thickBot="1">
+      <c r="K41" s="30"/>
+      <c r="M41">
+        <v>0</v>
+      </c>
+      <c r="U41" s="30"/>
+      <c r="W41">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="11:23" ht="15.75" thickBot="1">
+      <c r="K42" s="2"/>
+      <c r="M42" t="s">
+        <v>22</v>
+      </c>
+      <c r="U42" s="2"/>
+      <c r="W42" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="43" spans="11:23" ht="15.75" thickBot="1">
+      <c r="K43" s="31"/>
+      <c r="M43" t="s">
+        <v>23</v>
+      </c>
+      <c r="U43" s="31"/>
+      <c r="W43" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="50" spans="8:37">
+      <c r="AH50" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="51" spans="8:37" ht="15.75" thickBot="1"/>
+    <row r="52" spans="8:37" ht="15.75" thickBot="1">
+      <c r="AH52" s="30"/>
+      <c r="AJ52">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="8:37" ht="15.75" thickBot="1">
+      <c r="AH53" s="2"/>
+      <c r="AJ53" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="54" spans="8:37" ht="15.75" thickBot="1">
+      <c r="V54" t="s">
+        <v>26</v>
+      </c>
+      <c r="AH54" s="31"/>
+      <c r="AJ54" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="56" spans="8:37" ht="15.75" thickBot="1">
+      <c r="K56" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="57" spans="8:37" ht="15.75" thickBot="1">
+      <c r="H57" s="25"/>
+      <c r="I57" s="26"/>
+      <c r="J57" s="26"/>
+      <c r="K57" s="26"/>
+      <c r="L57" s="26"/>
+      <c r="M57" s="26"/>
+      <c r="N57" s="26"/>
+      <c r="O57" s="26"/>
+      <c r="P57" s="3"/>
+      <c r="Q57" s="25"/>
+      <c r="R57" s="26"/>
+      <c r="S57" s="26"/>
+      <c r="T57" s="26"/>
+      <c r="U57" s="26"/>
+      <c r="V57" s="26"/>
+      <c r="W57" s="26"/>
+      <c r="X57" s="26"/>
+      <c r="Y57" s="3"/>
+      <c r="Z57" s="26"/>
+      <c r="AA57" s="26"/>
+      <c r="AB57" s="26"/>
+      <c r="AC57" s="26"/>
+      <c r="AD57" s="26"/>
+      <c r="AE57" s="26"/>
+      <c r="AF57" s="26"/>
+      <c r="AG57" s="26"/>
+      <c r="AH57" s="3"/>
+      <c r="AK57" t="s">
+        <v>17</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48E9978B-894D-45BE-8A10-ACBB05A286EC}">
   <dimension ref="A1:I41"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G29" sqref="G29"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="V19" sqref="V19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>

<commit_message>
ex06 - p2 - code is a mess, but cg converges now most system assembly is still on cpu
</commit_message>
<xml_diff>
--- a/ex06/ex06.xlsx
+++ b/ex06/ex06.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\CSE\CSMC\CSMC_2021WS\ex06\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BF9FA92-7C4F-4676-87D1-9B8A28C7CA17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18E4657A-3B62-4C12-B99E-6C26DF8B7480}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="16080" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="16080" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Prefix sum" sheetId="3" r:id="rId1"/>
     <sheet name="Kernel1" sheetId="5" r:id="rId2"/>
     <sheet name="Part1_timings" sheetId="4" r:id="rId3"/>
+    <sheet name="P2_sanity" sheetId="6" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="32">
   <si>
     <t>grid level</t>
   </si>
@@ -126,6 +127,12 @@
   </si>
   <si>
     <t>stride = 4</t>
+  </si>
+  <si>
+    <t>sum</t>
+  </si>
+  <si>
+    <t>row offsets</t>
   </si>
 </sst>
 </file>
@@ -4496,7 +4503,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48E9978B-894D-45BE-8A10-ACBB05A286EC}">
   <dimension ref="A1:I41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+    <sheetView topLeftCell="D1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
       <selection activeCell="V19" sqref="V19"/>
     </sheetView>
   </sheetViews>
@@ -4971,4 +4978,111 @@
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19B62321-FE23-4D09-889C-C1CF036FBD72}">
+  <dimension ref="A1:O6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M20" sqref="M20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15">
+      <c r="O1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15">
+      <c r="B2" s="23">
+        <v>3</v>
+      </c>
+      <c r="C2">
+        <v>4</v>
+      </c>
+      <c r="D2">
+        <v>4</v>
+      </c>
+      <c r="E2">
+        <v>3</v>
+      </c>
+      <c r="F2">
+        <v>4</v>
+      </c>
+      <c r="G2">
+        <v>5</v>
+      </c>
+      <c r="H2">
+        <v>5</v>
+      </c>
+      <c r="I2">
+        <v>4</v>
+      </c>
+      <c r="J2">
+        <v>3</v>
+      </c>
+      <c r="K2">
+        <v>4</v>
+      </c>
+      <c r="L2">
+        <v>4</v>
+      </c>
+      <c r="M2">
+        <v>3</v>
+      </c>
+      <c r="O2">
+        <f>SUM(B2:M2)</f>
+        <v>46</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15">
+      <c r="A6" t="s">
+        <v>31</v>
+      </c>
+      <c r="B6" s="23">
+        <v>0</v>
+      </c>
+      <c r="C6">
+        <v>3</v>
+      </c>
+      <c r="D6">
+        <v>7</v>
+      </c>
+      <c r="E6">
+        <v>11</v>
+      </c>
+      <c r="F6">
+        <v>14</v>
+      </c>
+      <c r="G6">
+        <v>18</v>
+      </c>
+      <c r="H6">
+        <v>23</v>
+      </c>
+      <c r="I6">
+        <v>28</v>
+      </c>
+      <c r="J6">
+        <v>32</v>
+      </c>
+      <c r="K6">
+        <v>35</v>
+      </c>
+      <c r="L6">
+        <v>39</v>
+      </c>
+      <c r="M6">
+        <v>43</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
ex06 - p2 - benchmarking of system assembly done
</commit_message>
<xml_diff>
--- a/ex06/ex06.xlsx
+++ b/ex06/ex06.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\CSE\CSMC\CSMC_2021WS\ex06\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18E4657A-3B62-4C12-B99E-6C26DF8B7480}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2249CC99-D51E-4CC5-A1D1-F9A8465F82D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="16080" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="16080" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Prefix sum" sheetId="3" r:id="rId1"/>
     <sheet name="Kernel1" sheetId="5" r:id="rId2"/>
     <sheet name="Part1_timings" sheetId="4" r:id="rId3"/>
     <sheet name="P2_sanity" sheetId="6" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="7" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="35">
   <si>
     <t>grid level</t>
   </si>
@@ -133,6 +134,15 @@
   </si>
   <si>
     <t>row offsets</t>
+  </si>
+  <si>
+    <t>benchmarking system assembly</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> time device SA in s</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> time host SA in s</t>
   </si>
 </sst>
 </file>
@@ -1311,6 +1321,450 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$B$6</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v> time device SA in s</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$A$7:$A$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>900</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3600</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>14400</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>57600</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>230400</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>921600</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$B$7:$B$12</c:f>
+              <c:numCache>
+                <c:formatCode>0.00E+00</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>1.9699999999999999E-4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.3699999999999999E-4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.3100000000000001E-4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6.4499999999999996E-4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4.7699999999999999E-4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.7160000000000001E-3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-2FC8-4E0B-9D09-1C909165214F}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$C$6</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v> time host SA in s</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$A$7:$A$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>900</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3600</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>14400</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>57600</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>230400</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>921600</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$C$7:$C$12</c:f>
+              <c:numCache>
+                <c:formatCode>0.00E+00</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>1.792E-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7.737E-3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.8787000000000002E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.175399</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.75156800000000001</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.8961839999999999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-2FC8-4E0B-9D09-1C909165214F}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="2050230943"/>
+        <c:axId val="2050231775"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="2050230943"/>
+        <c:scaling>
+          <c:logBase val="10"/>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2050231775"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="2050231775"/>
+        <c:scaling>
+          <c:logBase val="10"/>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0.00E+00" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2050230943"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -1351,7 +1805,563 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -3283,6 +4293,47 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>581025</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>61912</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>276225</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>138112</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{87216A7E-F775-4DF7-95F8-5AA1082A675B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -4984,7 +6035,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19B62321-FE23-4D09-889C-C1CF036FBD72}">
   <dimension ref="A1:O6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="M20" sqref="M20"/>
     </sheetView>
   </sheetViews>
@@ -5085,4 +6136,103 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B80AF91-9DB9-4267-A85D-382AC1389184}">
+  <dimension ref="A5:C12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F24" sqref="F24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="5" spans="1:3">
+      <c r="A5" s="23" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" s="23" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" t="s">
+        <v>33</v>
+      </c>
+      <c r="C6" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" s="23">
+        <v>900</v>
+      </c>
+      <c r="B7" s="24">
+        <v>1.9699999999999999E-4</v>
+      </c>
+      <c r="C7" s="24">
+        <v>1.792E-3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" s="23">
+        <v>3600</v>
+      </c>
+      <c r="B8" s="24">
+        <v>2.3699999999999999E-4</v>
+      </c>
+      <c r="C8" s="24">
+        <v>7.737E-3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" s="23">
+        <v>14400</v>
+      </c>
+      <c r="B9" s="24">
+        <v>4.3100000000000001E-4</v>
+      </c>
+      <c r="C9" s="24">
+        <v>3.8787000000000002E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" s="23">
+        <v>57600</v>
+      </c>
+      <c r="B10" s="24">
+        <v>6.4499999999999996E-4</v>
+      </c>
+      <c r="C10" s="24">
+        <v>0.175399</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" s="23">
+        <v>230400</v>
+      </c>
+      <c r="B11" s="24">
+        <v>4.7699999999999999E-4</v>
+      </c>
+      <c r="C11" s="24">
+        <v>0.75156800000000001</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12" s="23">
+        <v>921600</v>
+      </c>
+      <c r="B12" s="24">
+        <v>1.7160000000000001E-3</v>
+      </c>
+      <c r="C12" s="24">
+        <v>2.8961839999999999</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
ex06 - coding done (i think)
</commit_message>
<xml_diff>
--- a/ex06/ex06.xlsx
+++ b/ex06/ex06.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\CSE\CSMC\CSMC_2021WS\ex06\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2249CC99-D51E-4CC5-A1D1-F9A8465F82D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B6A0752-9A5D-4665-9796-BB3D237464C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="16080" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="37">
   <si>
     <t>grid level</t>
   </si>
@@ -143,6 +143,12 @@
   </si>
   <si>
     <t xml:space="preserve"> time host SA in s</t>
+  </si>
+  <si>
+    <t>time for cg solver</t>
+  </si>
+  <si>
+    <t>grid size</t>
   </si>
 </sst>
 </file>
@@ -1335,37 +1341,7 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
-    <c:title>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
+    <c:autoTitleDeleted val="1"/>
     <c:plotArea>
       <c:layout/>
       <c:scatterChart>
@@ -1376,7 +1352,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$B$6</c:f>
+              <c:f>Sheet1!$C$6</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1399,7 +1375,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$7:$A$12</c:f>
+              <c:f>Sheet1!$B$7:$B$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -1426,7 +1402,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$B$7:$B$12</c:f>
+              <c:f>Sheet1!$C$7:$C$12</c:f>
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="6"/>
@@ -1463,7 +1439,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$C$6</c:f>
+              <c:f>Sheet1!$D$6</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1486,7 +1462,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$7:$A$12</c:f>
+              <c:f>Sheet1!$B$7:$B$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -1513,7 +1489,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$C$7:$C$12</c:f>
+              <c:f>Sheet1!$D$7:$D$12</c:f>
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="6"/>
@@ -1542,6 +1518,93 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-2FC8-4E0B-9D09-1C909165214F}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$E$6</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>time for cg solver</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$B$7:$B$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>900</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3600</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>14400</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>57600</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>230400</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>921600</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$E$7:$E$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>8.5249999999999996E-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.6493000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.5187999999999997E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.12673400000000001</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.59076399999999996</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.03868</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-2FC8-4E0B-9D09-1C909165214F}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1561,6 +1624,7 @@
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
+          <c:min val="100"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
@@ -1578,7 +1642,7 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="0.E+00" sourceLinked="0"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1616,7 +1680,7 @@
           </a:p>
         </c:txPr>
         <c:crossAx val="2050231775"/>
-        <c:crosses val="autoZero"/>
+        <c:crossesAt val="1.0000000000000003E-4"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
@@ -1641,7 +1705,7 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="0.00E+00" sourceLinked="1"/>
+        <c:numFmt formatCode="0.E+00" sourceLinked="0"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -4297,16 +4361,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>581025</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>61912</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>209550</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>71437</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>276225</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>138112</xdr:rowOff>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>514350</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>147637</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -6140,94 +6204,142 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B80AF91-9DB9-4267-A85D-382AC1389184}">
-  <dimension ref="A5:C12"/>
+  <dimension ref="A5:E12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F24" sqref="F24"/>
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:5">
       <c r="A5" s="23" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
-      <c r="A6" s="23" t="s">
+    <row r="6" spans="1:5">
+      <c r="A6" t="s">
+        <v>36</v>
+      </c>
+      <c r="B6" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C6" t="s">
         <v>33</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="7" spans="1:3">
-      <c r="A7" s="23">
+      <c r="E6" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7">
+        <f>SQRT(B7)</f>
+        <v>30</v>
+      </c>
+      <c r="B7" s="23">
         <v>900</v>
       </c>
-      <c r="B7" s="24">
+      <c r="C7" s="24">
         <v>1.9699999999999999E-4</v>
       </c>
-      <c r="C7" s="24">
+      <c r="D7" s="24">
         <v>1.792E-3</v>
       </c>
-    </row>
-    <row r="8" spans="1:3">
-      <c r="A8" s="23">
+      <c r="E7" s="23">
+        <v>8.5249999999999996E-3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8">
+        <f>SQRT(B8)</f>
+        <v>60</v>
+      </c>
+      <c r="B8" s="23">
         <v>3600</v>
       </c>
-      <c r="B8" s="24">
+      <c r="C8" s="24">
         <v>2.3699999999999999E-4</v>
       </c>
-      <c r="C8" s="24">
+      <c r="D8" s="24">
         <v>7.737E-3</v>
       </c>
-    </row>
-    <row r="9" spans="1:3">
-      <c r="A9" s="23">
+      <c r="E8" s="23">
+        <v>1.6493000000000001E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9">
+        <f>SQRT(B9)</f>
+        <v>120</v>
+      </c>
+      <c r="B9" s="23">
         <v>14400</v>
       </c>
-      <c r="B9" s="24">
+      <c r="C9" s="24">
         <v>4.3100000000000001E-4</v>
       </c>
-      <c r="C9" s="24">
+      <c r="D9" s="24">
         <v>3.8787000000000002E-2</v>
       </c>
-    </row>
-    <row r="10" spans="1:3">
-      <c r="A10" s="23">
+      <c r="E9" s="23">
+        <v>3.5187999999999997E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10">
+        <f>SQRT(B10)</f>
+        <v>240</v>
+      </c>
+      <c r="B10" s="23">
         <v>57600</v>
       </c>
-      <c r="B10" s="24">
+      <c r="C10" s="24">
         <v>6.4499999999999996E-4</v>
       </c>
-      <c r="C10" s="24">
+      <c r="D10" s="24">
         <v>0.175399</v>
       </c>
-    </row>
-    <row r="11" spans="1:3">
-      <c r="A11" s="23">
+      <c r="E10" s="23">
+        <v>0.12673400000000001</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11">
+        <f>SQRT(B11)</f>
+        <v>480</v>
+      </c>
+      <c r="B11" s="23">
         <v>230400</v>
       </c>
-      <c r="B11" s="24">
+      <c r="C11" s="24">
         <v>4.7699999999999999E-4</v>
       </c>
-      <c r="C11" s="24">
+      <c r="D11" s="24">
         <v>0.75156800000000001</v>
       </c>
-    </row>
-    <row r="12" spans="1:3">
-      <c r="A12" s="23">
+      <c r="E11" s="23">
+        <v>0.59076399999999996</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12">
+        <f>SQRT(B12)</f>
+        <v>960</v>
+      </c>
+      <c r="B12" s="23">
         <v>921600</v>
       </c>
-      <c r="B12" s="24">
+      <c r="C12" s="24">
         <v>1.7160000000000001E-3</v>
       </c>
-      <c r="C12" s="24">
+      <c r="D12" s="24">
         <v>2.8961839999999999</v>
+      </c>
+      <c r="E12" s="23">
+        <v>1.03868</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
ex06 - documentation main part is done - bonus point is missing
</commit_message>
<xml_diff>
--- a/ex06/ex06.xlsx
+++ b/ex06/ex06.xlsx
@@ -8,16 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\CSE\CSMC\CSMC_2021WS\ex06\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B6A0752-9A5D-4665-9796-BB3D237464C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BCAB3D8-B020-4A11-8A97-4587417625B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="16080" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="16080" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Prefix sum" sheetId="3" r:id="rId1"/>
     <sheet name="Kernel1" sheetId="5" r:id="rId2"/>
     <sheet name="Part1_timings" sheetId="4" r:id="rId3"/>
-    <sheet name="P2_sanity" sheetId="6" r:id="rId4"/>
-    <sheet name="Sheet1" sheetId="7" r:id="rId5"/>
+    <sheet name="P2_Performance" sheetId="7" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -115,9 +114,6 @@
     <t>sum1 + sum2</t>
   </si>
   <si>
-    <t>already done</t>
-  </si>
-  <si>
     <t>add to each entry</t>
   </si>
   <si>
@@ -128,12 +124,6 @@
   </si>
   <si>
     <t>stride = 4</t>
-  </si>
-  <si>
-    <t>sum</t>
-  </si>
-  <si>
-    <t>row offsets</t>
   </si>
   <si>
     <t>benchmarking system assembly</t>
@@ -149,6 +139,15 @@
   </si>
   <si>
     <t>grid size</t>
+  </si>
+  <si>
+    <t>GPU system assembly</t>
+  </si>
+  <si>
+    <t>CPU system assembly</t>
+  </si>
+  <si>
+    <t>CG solver</t>
   </si>
 </sst>
 </file>
@@ -1248,10 +1247,10 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.19319588698284326"/>
-          <c:y val="9.4405429080520409E-2"/>
+          <c:x val="0.15653913420628132"/>
+          <c:y val="5.489926238564987E-2"/>
           <c:w val="0.29781386701662299"/>
-          <c:h val="0.31584153734359288"/>
+          <c:h val="0.2644835206402612"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="0"/>
@@ -1267,7 +1266,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+            <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1">
                   <a:lumMod val="65000"/>
@@ -1343,7 +1342,17 @@
   <c:chart>
     <c:autoTitleDeleted val="1"/>
     <c:plotArea>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.16872107207622022"/>
+          <c:y val="5.0925925925925923E-2"/>
+          <c:w val="0.76639330847068532"/>
+          <c:h val="0.76626749781277337"/>
+        </c:manualLayout>
+      </c:layout>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
         <c:varyColors val="0"/>
@@ -1352,11 +1361,11 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$C$6</c:f>
+              <c:f>P2_Performance!$C$6</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v> time device SA in s</c:v>
+                  <c:v>GPU system assembly</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1371,11 +1380,23 @@
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="none"/>
+            <c:symbol val="triangle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$B$7:$B$12</c:f>
+              <c:f>P2_Performance!$B$7:$B$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -1402,7 +1423,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$C$7:$C$12</c:f>
+              <c:f>P2_Performance!$C$7:$C$12</c:f>
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="6"/>
@@ -1439,11 +1460,11 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$D$6</c:f>
+              <c:f>P2_Performance!$D$6</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v> time host SA in s</c:v>
+                  <c:v>CPU system assembly</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1458,11 +1479,23 @@
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="none"/>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$B$7:$B$12</c:f>
+              <c:f>P2_Performance!$B$7:$B$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -1489,7 +1522,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$D$7:$D$12</c:f>
+              <c:f>P2_Performance!$D$7:$D$12</c:f>
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="6"/>
@@ -1526,11 +1559,11 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$E$6</c:f>
+              <c:f>P2_Performance!$E$6</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>time for cg solver</c:v>
+                  <c:v>CG solver</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1545,11 +1578,23 @@
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="none"/>
+            <c:symbol val="square"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$B$7:$B$12</c:f>
+              <c:f>P2_Performance!$B$7:$B$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -1576,7 +1621,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$E$7:$E$12</c:f>
+              <c:f>P2_Performance!$E$7:$E$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -1642,6 +1687,61 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>number of unknowns</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="0.E+00" sourceLinked="0"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -1705,6 +1805,61 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>execution time in s</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="0.E+00" sourceLinked="0"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -1756,6 +1911,16 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.1729523776271083"/>
+          <c:y val="5.150408282298042E-2"/>
+          <c:w val="0.36032610949021393"/>
+          <c:h val="0.30960702828813058"/>
+        </c:manualLayout>
+      </c:layout>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1769,7 +1934,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+            <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1">
                   <a:lumMod val="65000"/>
@@ -3679,13 +3844,13 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>14</xdr:col>
-      <xdr:colOff>20839</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>47626</xdr:rowOff>
+      <xdr:colOff>20840</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>184547</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>17</xdr:col>
-      <xdr:colOff>5955</xdr:colOff>
+      <xdr:colOff>5956</xdr:colOff>
       <xdr:row>13</xdr:row>
       <xdr:rowOff>181572</xdr:rowOff>
     </xdr:to>
@@ -3702,8 +3867,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm rot="16200000">
-          <a:off x="2714628" y="2330650"/>
-          <a:ext cx="133946" cy="520897"/>
+          <a:off x="2687839" y="2303861"/>
+          <a:ext cx="187525" cy="520897"/>
         </a:xfrm>
         <a:prstGeom prst="rightBrace">
           <a:avLst/>
@@ -3742,15 +3907,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>2</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>35719</xdr:rowOff>
+      <xdr:colOff>17861</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>29765</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>31</xdr:col>
-      <xdr:colOff>142875</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>47625</xdr:rowOff>
+      <xdr:colOff>160734</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>154780</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -3765,11 +3930,14 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm rot="16200000">
-          <a:off x="3184923" y="-160733"/>
-          <a:ext cx="202406" cy="4786310"/>
+          <a:off x="3146227" y="-300632"/>
+          <a:ext cx="315515" cy="4786310"/>
         </a:xfrm>
         <a:prstGeom prst="rightBrace">
-          <a:avLst/>
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 8333"/>
+            <a:gd name="adj2" fmla="val 49876"/>
+          </a:avLst>
         </a:prstGeom>
         <a:ln w="12700">
           <a:solidFill>
@@ -4035,16 +4203,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>119062</xdr:colOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>125016</xdr:colOff>
       <xdr:row>23</xdr:row>
-      <xdr:rowOff>83345</xdr:rowOff>
+      <xdr:rowOff>113109</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>30</xdr:col>
-      <xdr:colOff>172640</xdr:colOff>
+      <xdr:colOff>142874</xdr:colOff>
       <xdr:row>26</xdr:row>
-      <xdr:rowOff>184546</xdr:rowOff>
+      <xdr:rowOff>154782</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -4059,8 +4227,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipV="1">
-          <a:off x="1905000" y="4512470"/>
-          <a:ext cx="3625453" cy="696514"/>
+          <a:off x="2089547" y="4542234"/>
+          <a:ext cx="3411140" cy="636986"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -4091,16 +4259,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>130968</xdr:colOff>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>71438</xdr:colOff>
       <xdr:row>24</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
+      <xdr:rowOff>101203</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>31</xdr:col>
-      <xdr:colOff>11906</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>5953</xdr:rowOff>
+      <xdr:col>30</xdr:col>
+      <xdr:colOff>136921</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>160735</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -4115,8 +4283,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipV="1">
-          <a:off x="3345656" y="4726781"/>
-          <a:ext cx="2202656" cy="506016"/>
+          <a:off x="3464719" y="4732734"/>
+          <a:ext cx="2030015" cy="452439"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -4285,6 +4453,62 @@
         <a:xfrm flipH="1">
           <a:off x="5464969" y="10465594"/>
           <a:ext cx="363140" cy="351234"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="25400">
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+          <a:tailEnd type="arrow" w="med" len="med"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>130968</xdr:colOff>
+      <xdr:row>51</xdr:row>
+      <xdr:rowOff>140494</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>32</xdr:col>
+      <xdr:colOff>122635</xdr:colOff>
+      <xdr:row>55</xdr:row>
+      <xdr:rowOff>130968</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="17" name="Straight Arrow Connector 16">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0F80BC1F-D15B-43AC-B2B1-F7DC9FC45285}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="2631281" y="10034588"/>
+          <a:ext cx="3206354" cy="788193"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -4361,16 +4585,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>209550</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>71437</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>390525</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>138112</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>514350</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>147637</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>85725</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>23812</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4663,7 +4887,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F3F8FFA-9A53-4E7A-B7DD-1557C851762A}">
   <dimension ref="H4:BA38"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="D3" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="AG18" sqref="AG18"/>
     </sheetView>
   </sheetViews>
@@ -4766,7 +4990,7 @@
       <c r="AW6" s="19"/>
       <c r="AX6" s="7"/>
       <c r="BA6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="7" spans="8:53" ht="15.75" thickBot="1"/>
@@ -4849,7 +5073,7 @@
       <c r="AW11" s="19"/>
       <c r="AX11" s="7"/>
       <c r="BA11" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="12" spans="8:53" ht="15.75" thickBot="1">
@@ -4980,7 +5204,7 @@
       <c r="AW16" s="19"/>
       <c r="AX16" s="7"/>
       <c r="BA16" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="17" spans="8:50" ht="15.75" thickBot="1"/>
@@ -5168,8 +5392,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FBDD1BDF-C854-4E6E-A40A-935551068A3F}">
   <dimension ref="F4:AQ57"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="W41" sqref="W41"/>
+    <sheetView showGridLines="0" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="AV46" sqref="AV46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.7109375" defaultRowHeight="15"/>
@@ -5373,8 +5597,8 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="6:43">
-      <c r="S11" s="29" t="s">
+    <row r="10" spans="6:43">
+      <c r="S10" s="29" t="s">
         <v>14</v>
       </c>
     </row>
@@ -5557,25 +5781,21 @@
       </c>
     </row>
     <row r="53" spans="8:37" ht="15.75" thickBot="1">
+      <c r="T53" t="s">
+        <v>25</v>
+      </c>
       <c r="AH53" s="2"/>
       <c r="AJ53" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="54" spans="8:37" ht="15.75" thickBot="1">
-      <c r="V54" t="s">
-        <v>26</v>
-      </c>
       <c r="AH54" s="31"/>
       <c r="AJ54" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="56" spans="8:37" ht="15.75" thickBot="1">
-      <c r="K56" t="s">
-        <v>25</v>
-      </c>
-    </row>
+    <row r="56" spans="8:37" ht="15.75" thickBot="1"/>
     <row r="57" spans="8:37" ht="15.75" thickBot="1">
       <c r="H57" s="25"/>
       <c r="I57" s="26"/>
@@ -5619,7 +5839,7 @@
   <dimension ref="A1:I41"/>
   <sheetViews>
     <sheetView topLeftCell="D1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="V19" sqref="V19"/>
+      <selection activeCell="U11" sqref="U11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -6096,147 +6316,49 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19B62321-FE23-4D09-889C-C1CF036FBD72}">
-  <dimension ref="A1:O6"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M20" sqref="M20"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:15">
-      <c r="O1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="2" spans="1:15">
-      <c r="B2" s="23">
-        <v>3</v>
-      </c>
-      <c r="C2">
-        <v>4</v>
-      </c>
-      <c r="D2">
-        <v>4</v>
-      </c>
-      <c r="E2">
-        <v>3</v>
-      </c>
-      <c r="F2">
-        <v>4</v>
-      </c>
-      <c r="G2">
-        <v>5</v>
-      </c>
-      <c r="H2">
-        <v>5</v>
-      </c>
-      <c r="I2">
-        <v>4</v>
-      </c>
-      <c r="J2">
-        <v>3</v>
-      </c>
-      <c r="K2">
-        <v>4</v>
-      </c>
-      <c r="L2">
-        <v>4</v>
-      </c>
-      <c r="M2">
-        <v>3</v>
-      </c>
-      <c r="O2">
-        <f>SUM(B2:M2)</f>
-        <v>46</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15">
-      <c r="A6" t="s">
-        <v>31</v>
-      </c>
-      <c r="B6" s="23">
-        <v>0</v>
-      </c>
-      <c r="C6">
-        <v>3</v>
-      </c>
-      <c r="D6">
-        <v>7</v>
-      </c>
-      <c r="E6">
-        <v>11</v>
-      </c>
-      <c r="F6">
-        <v>14</v>
-      </c>
-      <c r="G6">
-        <v>18</v>
-      </c>
-      <c r="H6">
-        <v>23</v>
-      </c>
-      <c r="I6">
-        <v>28</v>
-      </c>
-      <c r="J6">
-        <v>32</v>
-      </c>
-      <c r="K6">
-        <v>35</v>
-      </c>
-      <c r="L6">
-        <v>39</v>
-      </c>
-      <c r="M6">
-        <v>43</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B80AF91-9DB9-4267-A85D-382AC1389184}">
   <dimension ref="A5:E12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="P3" sqref="P3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="5" spans="1:5">
       <c r="A5" s="23" t="s">
+        <v>29</v>
+      </c>
+      <c r="C5" t="s">
+        <v>30</v>
+      </c>
+      <c r="D5" t="s">
+        <v>31</v>
+      </c>
+      <c r="E5" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B6" s="23" t="s">
         <v>12</v>
       </c>
       <c r="C6" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D6" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E6" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="7" spans="1:5">
       <c r="A7">
-        <f>SQRT(B7)</f>
+        <f t="shared" ref="A7:A12" si="0">SQRT(B7)</f>
         <v>30</v>
       </c>
       <c r="B7" s="23">
@@ -6254,7 +6376,7 @@
     </row>
     <row r="8" spans="1:5">
       <c r="A8">
-        <f>SQRT(B8)</f>
+        <f t="shared" si="0"/>
         <v>60</v>
       </c>
       <c r="B8" s="23">
@@ -6272,7 +6394,7 @@
     </row>
     <row r="9" spans="1:5">
       <c r="A9">
-        <f>SQRT(B9)</f>
+        <f t="shared" si="0"/>
         <v>120</v>
       </c>
       <c r="B9" s="23">
@@ -6290,7 +6412,7 @@
     </row>
     <row r="10" spans="1:5">
       <c r="A10">
-        <f>SQRT(B10)</f>
+        <f t="shared" si="0"/>
         <v>240</v>
       </c>
       <c r="B10" s="23">
@@ -6308,7 +6430,7 @@
     </row>
     <row r="11" spans="1:5">
       <c r="A11">
-        <f>SQRT(B11)</f>
+        <f t="shared" si="0"/>
         <v>480</v>
       </c>
       <c r="B11" s="23">
@@ -6326,7 +6448,7 @@
     </row>
     <row r="12" spans="1:5">
       <c r="A12">
-        <f>SQRT(B12)</f>
+        <f t="shared" si="0"/>
         <v>960</v>
       </c>
       <c r="B12" s="23">

</xml_diff>